<commit_message>
new analysis models cleaner
</commit_message>
<xml_diff>
--- a/data/Data Proxy Industrializtaion/Berufsstatistik Sachsen 1861.xlsx
+++ b/data/Data Proxy Industrializtaion/Berufsstatistik Sachsen 1861.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasoedekoven/Desktop/Masterarbeit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasoedekoven/Desktop/Masterarbeit All/Gellner/data/Data Proxy Industrializtaion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B819E686-0F65-F045-9697-8942BE220D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEF4BDD-2874-BF4D-81F7-BD673CAA10E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28740" windowHeight="16400" xr2:uid="{A9F2E1ED-BA03-D042-8731-3BC558C98A17}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Berufst. Sachsen" sheetId="2" r:id="rId1"/>
     <sheet name="Codebook" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Berufst. Sachsen'!$A$1:$AS$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="197">
   <si>
     <t>Citykey</t>
   </si>
@@ -185,108 +188,54 @@
     <t>se_agr_for</t>
   </si>
   <si>
-    <t>emp_agr_for</t>
-  </si>
-  <si>
     <t>se_min</t>
   </si>
   <si>
-    <t>emp_min</t>
-  </si>
-  <si>
     <t>se_craft</t>
   </si>
   <si>
-    <t>emp_craft</t>
-  </si>
-  <si>
     <t>se_fac_man</t>
   </si>
   <si>
-    <t>emp_fac_man</t>
-  </si>
-  <si>
     <t>sum_ind</t>
   </si>
   <si>
     <t>se_trd</t>
   </si>
   <si>
-    <t>emp_trd</t>
-  </si>
-  <si>
     <t>se_litrd</t>
   </si>
   <si>
-    <t>emp_litrd</t>
-  </si>
-  <si>
     <t>se_pas_carg_pos</t>
   </si>
   <si>
-    <t>emp_pas_carg_pos</t>
-  </si>
-  <si>
-    <t>sum_trd_ser</t>
-  </si>
-  <si>
     <t>se_ad_jud</t>
   </si>
   <si>
-    <t>emp_ad_jud</t>
-  </si>
-  <si>
     <t>se_hea</t>
   </si>
   <si>
-    <t>emp_hea</t>
-  </si>
-  <si>
     <t>se_edu</t>
   </si>
   <si>
-    <t>emp_edu</t>
-  </si>
-  <si>
     <t>se_art</t>
   </si>
   <si>
-    <t>emp_art</t>
-  </si>
-  <si>
     <t>se_arm</t>
   </si>
   <si>
-    <t>emp_arm</t>
-  </si>
-  <si>
     <t>se_cor</t>
   </si>
   <si>
-    <t>emp_cor</t>
-  </si>
-  <si>
     <t>se_hou</t>
   </si>
   <si>
-    <t>emp_hou</t>
-  </si>
-  <si>
-    <t>sum_IV</t>
-  </si>
-  <si>
     <t>se_oth</t>
   </si>
   <si>
-    <t>emp_oth</t>
-  </si>
-  <si>
     <t>se_sum</t>
   </si>
   <si>
-    <t>emp_sum</t>
-  </si>
-  <si>
     <t>Dippoldiswalde</t>
   </si>
   <si>
@@ -296,21 +245,12 @@
     <t>se_sum_ind</t>
   </si>
   <si>
-    <t>emp_sum_ind</t>
-  </si>
-  <si>
     <t>se_sum_trd_ser</t>
   </si>
   <si>
-    <t>emp_sum_trd_ser</t>
-  </si>
-  <si>
     <t>se_sum_IV</t>
   </si>
   <si>
-    <t>emp_sum_IV</t>
-  </si>
-  <si>
     <t>sum</t>
   </si>
   <si>
@@ -624,6 +564,72 @@
   </si>
   <si>
     <t>cityname</t>
+  </si>
+  <si>
+    <t>rel_agr_for</t>
+  </si>
+  <si>
+    <t>rel_min</t>
+  </si>
+  <si>
+    <t>rel_craft</t>
+  </si>
+  <si>
+    <t>rel_fac_man</t>
+  </si>
+  <si>
+    <t>rel_sum_ind</t>
+  </si>
+  <si>
+    <t>rel_trd</t>
+  </si>
+  <si>
+    <t>rel_litrd</t>
+  </si>
+  <si>
+    <t>_pas_carg_pos</t>
+  </si>
+  <si>
+    <t>rel_sum_trd_ser</t>
+  </si>
+  <si>
+    <t>rel_ad_jud</t>
+  </si>
+  <si>
+    <t>rel_hea</t>
+  </si>
+  <si>
+    <t>rel_edu</t>
+  </si>
+  <si>
+    <t>rel_art</t>
+  </si>
+  <si>
+    <t>rel_arm</t>
+  </si>
+  <si>
+    <t>rel_cor</t>
+  </si>
+  <si>
+    <t>rel_hou</t>
+  </si>
+  <si>
+    <t>rel_sum_IV</t>
+  </si>
+  <si>
+    <t>rel_oth</t>
+  </si>
+  <si>
+    <t>rel_sum</t>
+  </si>
+  <si>
+    <t>rel_pas_carg_pos</t>
+  </si>
+  <si>
+    <t>Angehörige / rel:</t>
+  </si>
+  <si>
+    <t>Familienangehörige</t>
   </si>
 </sst>
 </file>
@@ -659,11 +665,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,7 +991,7 @@
   <dimension ref="A1:AS104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1007,136 +1016,136 @@
         <v>48</v>
       </c>
       <c r="G1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>179</v>
+      </c>
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
+        <v>180</v>
+      </c>
+      <c r="R1" t="s">
         <v>54</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
+        <v>181</v>
+      </c>
+      <c r="T1" t="s">
         <v>55</v>
       </c>
-      <c r="N1" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V1" t="s">
+        <v>68</v>
+      </c>
+      <c r="W1" t="s">
+        <v>183</v>
+      </c>
+      <c r="X1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z1" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AA1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB1" t="s">
         <v>58</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AC1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD1" t="s">
         <v>59</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF1" t="s">
         <v>60</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AG1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AH1" t="s">
         <v>61</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AI1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>62</v>
       </c>
-      <c r="V1" t="s">
-        <v>87</v>
-      </c>
-      <c r="W1" t="s">
-        <v>88</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="AK1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AP1" t="s">
         <v>64</v>
       </c>
-      <c r="Y1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="AQ1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AR1" t="s">
         <v>70</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AS1" t="s">
         <v>71</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B2,"Ä","Ae"),"Ö","Oe"),"Ü","Ue"),"ß","ss"),"ä","ae"),"ö","oe"),"ü","ue")</f>
         <v>Dippoldiswalde</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F2">
         <v>156</v>
@@ -1263,17 +1272,17 @@
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C66" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B3,"Ä","Ae"),"Ö","Oe"),"Ü","Ue"),"ß","ss"),"ä","ae"),"ö","oe"),"ü","ue")</f>
         <v>Dresden</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F3">
         <v>1032</v>
@@ -1400,17 +1409,17 @@
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="2"/>
         <v>Radeberg</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F4">
         <v>120</v>
@@ -1537,17 +1546,17 @@
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="2"/>
         <v>Radeburg</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F5">
         <v>180</v>
@@ -1674,17 +1683,17 @@
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="2"/>
         <v>Wilsdruff</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F6">
         <v>156</v>
@@ -1811,17 +1820,17 @@
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="2"/>
         <v>Grossenhain</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F7">
         <v>143</v>
@@ -1948,17 +1957,17 @@
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="2"/>
         <v>Lommatzsch</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F8">
         <v>29</v>
@@ -2085,17 +2094,17 @@
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="2"/>
         <v>Meissen</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F9">
         <v>84</v>
@@ -2222,17 +2231,17 @@
     </row>
     <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="2"/>
         <v>Nossen</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F10">
         <v>69</v>
@@ -2359,17 +2368,17 @@
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="2"/>
         <v>Riesa</v>
       </c>
       <c r="D11" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F11">
         <v>270</v>
@@ -2496,17 +2505,17 @@
     </row>
     <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="2"/>
         <v>Gottleuba</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F12">
         <v>143</v>
@@ -2633,17 +2642,17 @@
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="2"/>
         <v>Koenigstein</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F13">
         <v>85</v>
@@ -2770,17 +2779,17 @@
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="2"/>
         <v>Lauenstein</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F14">
         <v>317</v>
@@ -2907,17 +2916,17 @@
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="2"/>
         <v>Neustadt</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F15">
         <v>84</v>
@@ -3044,17 +3053,17 @@
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="2"/>
         <v>Pirna</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F16">
         <v>482</v>
@@ -3181,17 +3190,17 @@
     </row>
     <row r="17" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="2"/>
         <v>Schandau</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F17">
         <v>135</v>
@@ -3318,17 +3327,17 @@
     </row>
     <row r="18" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="2"/>
         <v>Sebnitz</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F18">
         <v>103</v>
@@ -3455,17 +3464,17 @@
     </row>
     <row r="19" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="2"/>
         <v>Stolpen</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F19">
         <v>45</v>
@@ -3592,17 +3601,17 @@
     </row>
     <row r="20" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="2"/>
         <v>Altenberg</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F20">
         <v>96</v>
@@ -3729,17 +3738,17 @@
     </row>
     <row r="21" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="2"/>
         <v>Brand</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F21">
         <v>26</v>
@@ -3866,17 +3875,17 @@
     </row>
     <row r="22" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="2"/>
         <v>Frauenstein</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F22">
         <v>106</v>
@@ -4003,17 +4012,17 @@
     </row>
     <row r="23" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="2"/>
         <v>Freiberg</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F23">
         <v>290</v>
@@ -4140,17 +4149,17 @@
     </row>
     <row r="24" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="2"/>
         <v>Sayda</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F24">
         <v>85</v>
@@ -4277,17 +4286,17 @@
     </row>
     <row r="25" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="2"/>
         <v>Tharandt</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F25">
         <v>152</v>
@@ -4414,17 +4423,17 @@
     </row>
     <row r="26" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="2"/>
         <v>Borna</v>
       </c>
       <c r="D26" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F26">
         <v>172</v>
@@ -4551,17 +4560,17 @@
     </row>
     <row r="27" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="2"/>
         <v>Leipzig</v>
       </c>
       <c r="D27" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E27" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F27">
         <v>263</v>
@@ -4688,17 +4697,17 @@
     </row>
     <row r="28" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="2"/>
         <v>Markranstaedt</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F28">
         <v>169</v>
@@ -4825,17 +4834,17 @@
     </row>
     <row r="29" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="2"/>
         <v>Pegau</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F29">
         <v>107</v>
@@ -4962,17 +4971,17 @@
     </row>
     <row r="30" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="2"/>
         <v>Roetha</v>
       </c>
       <c r="D30" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F30">
         <v>130</v>
@@ -5099,17 +5108,17 @@
     </row>
     <row r="31" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="2"/>
         <v>Taucha</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F31">
         <v>123</v>
@@ -5236,17 +5245,17 @@
     </row>
     <row r="32" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="2"/>
         <v>Zwenkau</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="E32" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F32">
         <v>123</v>
@@ -5373,17 +5382,17 @@
     </row>
     <row r="33" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="2"/>
         <v>Brandis</v>
       </c>
       <c r="D33" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E33" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F33">
         <v>340</v>
@@ -5510,17 +5519,17 @@
     </row>
     <row r="34" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="2"/>
         <v>Grimma</v>
       </c>
       <c r="D34" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E34" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F34">
         <v>471</v>
@@ -5647,17 +5656,17 @@
     </row>
     <row r="35" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="2"/>
         <v>Lausigk</v>
       </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E35" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F35">
         <v>86</v>
@@ -5784,17 +5793,17 @@
     </row>
     <row r="36" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="2"/>
         <v>Oschatz</v>
       </c>
       <c r="D36" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F36">
         <v>611</v>
@@ -5921,17 +5930,17 @@
     </row>
     <row r="37" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="2"/>
         <v>Strehla</v>
       </c>
       <c r="D37" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E37" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F37">
         <v>82</v>
@@ -6058,17 +6067,17 @@
     </row>
     <row r="38" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="2"/>
         <v>Wermsdorf</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E38" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F38">
         <v>88</v>
@@ -6195,17 +6204,17 @@
     </row>
     <row r="39" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="2"/>
         <v>Wurzen</v>
       </c>
       <c r="D39" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F39">
         <v>96</v>
@@ -6332,17 +6341,17 @@
     </row>
     <row r="40" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="2"/>
         <v>Burgstaedt</v>
       </c>
       <c r="D40" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E40" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F40">
         <v>20</v>
@@ -6469,17 +6478,17 @@
     </row>
     <row r="41" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="2"/>
         <v>Colditz</v>
       </c>
       <c r="D41" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E41" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F41">
         <v>65</v>
@@ -6606,17 +6615,17 @@
     </row>
     <row r="42" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="2"/>
         <v>Frohburg</v>
       </c>
       <c r="D42" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F42">
         <v>109</v>
@@ -6743,17 +6752,17 @@
     </row>
     <row r="43" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="2"/>
         <v>Geithain</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E43" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F43">
         <v>215</v>
@@ -6880,17 +6889,17 @@
     </row>
     <row r="44" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="2"/>
         <v>Mittwieda</v>
       </c>
       <c r="D44" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E44" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F44">
         <v>72</v>
@@ -7017,17 +7026,17 @@
     </row>
     <row r="45" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="2"/>
         <v>Penig</v>
       </c>
       <c r="D45" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F45">
         <v>168</v>
@@ -7154,17 +7163,17 @@
     </row>
     <row r="46" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="2"/>
         <v>Rochlitz</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E46" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F46">
         <v>85</v>
@@ -7291,17 +7300,17 @@
     </row>
     <row r="47" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="2"/>
         <v>Doebeln</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E47" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F47">
         <v>96</v>
@@ -7428,17 +7437,17 @@
     </row>
     <row r="48" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="2"/>
         <v>Geringswalde</v>
       </c>
       <c r="D48" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E48" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F48">
         <v>52</v>
@@ -7565,17 +7574,17 @@
     </row>
     <row r="49" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="2"/>
         <v>Hainichen</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F49">
         <v>22</v>
@@ -7702,17 +7711,17 @@
     </row>
     <row r="50" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="2"/>
         <v>Hartha</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E50" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F50">
         <v>61</v>
@@ -7839,17 +7848,17 @@
     </row>
     <row r="51" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="2"/>
         <v>Leisnig</v>
       </c>
       <c r="D51" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E51" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F51">
         <v>79</v>
@@ -7976,17 +7985,17 @@
     </row>
     <row r="52" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="2"/>
         <v>Muegeln</v>
       </c>
       <c r="D52" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E52" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F52">
         <v>61</v>
@@ -8113,17 +8122,17 @@
     </row>
     <row r="53" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="2"/>
         <v>Rosswein</v>
       </c>
       <c r="D53" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E53" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F53">
         <v>74</v>
@@ -8250,17 +8259,17 @@
     </row>
     <row r="54" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="2"/>
         <v>Waldheim</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E54" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F54">
         <v>31</v>
@@ -8387,17 +8396,17 @@
     </row>
     <row r="55" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="2"/>
         <v>Augustusburg</v>
       </c>
       <c r="D55" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="E55" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F55">
         <v>37</v>
@@ -8524,17 +8533,17 @@
     </row>
     <row r="56" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="2"/>
         <v>Chemnitz</v>
       </c>
       <c r="D56" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="E56" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F56">
         <v>236</v>
@@ -8661,17 +8670,17 @@
     </row>
     <row r="57" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="2"/>
         <v>Frankenberg</v>
       </c>
       <c r="D57" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="E57" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F57">
         <v>80</v>
@@ -8798,17 +8807,17 @@
     </row>
     <row r="58" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="2"/>
         <v>Dederan</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F58">
         <v>45</v>
@@ -8935,17 +8944,17 @@
     </row>
     <row r="59" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="2"/>
         <v>Stollberg</v>
       </c>
       <c r="D59" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="E59" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F59">
         <v>107</v>
@@ -9072,17 +9081,17 @@
     </row>
     <row r="60" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="2"/>
         <v>Zschopau</v>
       </c>
       <c r="D60" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="E60" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F60">
         <v>97</v>
@@ -9209,17 +9218,17 @@
     </row>
     <row r="61" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="2"/>
         <v>Crimmitschau</v>
       </c>
       <c r="D61" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E61" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F61">
         <v>59</v>
@@ -9346,17 +9355,17 @@
     </row>
     <row r="62" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="2"/>
         <v>Eibenstock</v>
       </c>
       <c r="D62" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E62" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F62">
         <v>184</v>
@@ -9483,17 +9492,17 @@
     </row>
     <row r="63" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="2"/>
         <v>Johanngeorgenstadt</v>
       </c>
       <c r="D63" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E63" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F63">
         <v>56</v>
@@ -9620,17 +9629,17 @@
     </row>
     <row r="64" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="2"/>
         <v>Kirchberg</v>
       </c>
       <c r="D64" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E64" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F64">
         <v>61</v>
@@ -9757,17 +9766,17 @@
     </row>
     <row r="65" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="2"/>
         <v>Schneeberg</v>
       </c>
       <c r="D65" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E65" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F65">
         <v>215</v>
@@ -9894,17 +9903,17 @@
     </row>
     <row r="66" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="2"/>
         <v>Schwarzenberg</v>
       </c>
       <c r="D66" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E66" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F66">
         <v>121</v>
@@ -10031,17 +10040,17 @@
     </row>
     <row r="67" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" ref="C67:C104" si="6">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B67,"Ä","Ae"),"Ö","Oe"),"Ü","Ue"),"ß","ss"),"ä","ae"),"ö","oe"),"ü","ue")</f>
         <v>Werdau</v>
       </c>
       <c r="D67" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E67" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F67">
         <v>93</v>
@@ -10168,17 +10177,17 @@
     </row>
     <row r="68" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="6"/>
         <v>Wildenfels</v>
       </c>
       <c r="D68" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E68" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F68">
         <v>55</v>
@@ -10305,17 +10314,17 @@
     </row>
     <row r="69" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="6"/>
         <v>Zwickau</v>
       </c>
       <c r="D69" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E69" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F69">
         <v>369</v>
@@ -10442,17 +10451,17 @@
     </row>
     <row r="70" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="6"/>
         <v>Annaberg</v>
       </c>
       <c r="D70" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E70" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F70">
         <v>132</v>
@@ -10579,17 +10588,17 @@
     </row>
     <row r="71" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="6"/>
         <v>Ehrenfriedersdorf</v>
       </c>
       <c r="D71" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E71" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F71">
         <v>251</v>
@@ -10716,17 +10725,17 @@
     </row>
     <row r="72" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="6"/>
         <v>Geyer</v>
       </c>
       <c r="D72" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E72" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F72">
         <v>121</v>
@@ -10853,17 +10862,17 @@
     </row>
     <row r="73" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="6"/>
         <v>Gruenhain</v>
       </c>
       <c r="D73" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E73" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F73">
         <v>395</v>
@@ -10990,17 +10999,17 @@
     </row>
     <row r="74" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="6"/>
         <v>Joehstadt</v>
       </c>
       <c r="D74" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E74" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F74">
         <v>49</v>
@@ -11127,17 +11136,17 @@
     </row>
     <row r="75" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="6"/>
         <v>Lengefeld</v>
       </c>
       <c r="D75" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E75" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F75">
         <v>101</v>
@@ -11264,17 +11273,17 @@
     </row>
     <row r="76" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="6"/>
         <v>Marienberg</v>
       </c>
       <c r="D76" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E76" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F76">
         <v>291</v>
@@ -11401,17 +11410,17 @@
     </row>
     <row r="77" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="6"/>
         <v>Oberwiesenthal</v>
       </c>
       <c r="D77" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E77" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F77">
         <v>182</v>
@@ -11538,17 +11547,17 @@
     </row>
     <row r="78" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="6"/>
         <v>Scheibenberg</v>
       </c>
       <c r="D78" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E78" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F78">
         <v>249</v>
@@ -11675,17 +11684,17 @@
     </row>
     <row r="79" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="6"/>
         <v>Wolkenstein</v>
       </c>
       <c r="D79" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E79" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F79">
         <v>78</v>
@@ -11812,17 +11821,17 @@
     </row>
     <row r="80" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="6"/>
         <v>Zoeblitz</v>
       </c>
       <c r="D80" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="E80" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F80">
         <v>111</v>
@@ -11949,17 +11958,17 @@
     </row>
     <row r="81" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="6"/>
         <v>Adorf</v>
       </c>
       <c r="D81" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E81" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F81">
         <v>248</v>
@@ -12086,17 +12095,17 @@
     </row>
     <row r="82" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="6"/>
         <v>Auerbach</v>
       </c>
       <c r="D82" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E82" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F82">
         <v>58</v>
@@ -12223,17 +12232,17 @@
     </row>
     <row r="83" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="6"/>
         <v>Elsterberg</v>
       </c>
       <c r="D83" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E83" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F83">
         <v>34</v>
@@ -12360,17 +12369,17 @@
     </row>
     <row r="84" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="6"/>
         <v>Falkenstein</v>
       </c>
       <c r="D84" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E84" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F84">
         <v>41</v>
@@ -12497,17 +12506,17 @@
     </row>
     <row r="85" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="6"/>
         <v>Lengenfeld</v>
       </c>
       <c r="D85" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E85" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F85">
         <v>53</v>
@@ -12634,17 +12643,17 @@
     </row>
     <row r="86" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="6"/>
         <v>Markneukirchen</v>
       </c>
       <c r="D86" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E86" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F86">
         <v>79</v>
@@ -12771,17 +12780,17 @@
     </row>
     <row r="87" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="6"/>
         <v>Oelsnitz</v>
       </c>
       <c r="D87" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E87" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F87">
         <v>118</v>
@@ -12908,17 +12917,17 @@
     </row>
     <row r="88" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="6"/>
         <v>Pausa</v>
       </c>
       <c r="D88" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E88" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F88">
         <v>180</v>
@@ -13045,17 +13054,17 @@
     </row>
     <row r="89" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="6"/>
         <v>Plauen</v>
       </c>
       <c r="D89" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E89" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F89">
         <v>198</v>
@@ -13182,17 +13191,17 @@
     </row>
     <row r="90" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="6"/>
         <v>Reichenbach</v>
       </c>
       <c r="D90" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E90" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F90">
         <v>116</v>
@@ -13319,17 +13328,17 @@
     </row>
     <row r="91" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="6"/>
         <v>Schoeneck</v>
       </c>
       <c r="D91" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E91" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F91">
         <v>72</v>
@@ -13456,17 +13465,17 @@
     </row>
     <row r="92" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="6"/>
         <v>Treuen</v>
       </c>
       <c r="D92" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E92" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F92">
         <v>81</v>
@@ -13593,17 +13602,17 @@
     </row>
     <row r="93" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="6"/>
         <v>Bischofswerda</v>
       </c>
       <c r="D93" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="E93" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F93">
         <v>72</v>
@@ -13730,17 +13739,17 @@
     </row>
     <row r="94" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="6"/>
         <v>Budissin</v>
       </c>
       <c r="D94" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="E94" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F94">
         <v>203</v>
@@ -13867,17 +13876,17 @@
     </row>
     <row r="95" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="6"/>
         <v>Kamenz</v>
       </c>
       <c r="D95" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="E95" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F95">
         <v>196</v>
@@ -14004,17 +14013,17 @@
     </row>
     <row r="96" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="6"/>
         <v>Koenigsbrueck</v>
       </c>
       <c r="D96" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="E96" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F96">
         <v>59</v>
@@ -14141,17 +14150,17 @@
     </row>
     <row r="97" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="6"/>
         <v>Neufalza</v>
       </c>
       <c r="D97" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="E97" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F97">
         <v>11</v>
@@ -14278,17 +14287,17 @@
     </row>
     <row r="98" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="6"/>
         <v>Pulsnitz</v>
       </c>
       <c r="D98" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="E98" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F98">
         <v>60</v>
@@ -14405,7 +14414,7 @@
         <v>1240</v>
       </c>
       <c r="AR98">
-        <f t="shared" ref="AR98:AR129" si="7">SUM(AP98:AQ98)</f>
+        <f t="shared" ref="AR98:AR104" si="7">SUM(AP98:AQ98)</f>
         <v>2399</v>
       </c>
       <c r="AS98">
@@ -14415,17 +14424,17 @@
     </row>
     <row r="99" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="6"/>
         <v>Schirgiswalde</v>
       </c>
       <c r="D99" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="E99" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F99">
         <v>66</v>
@@ -14552,17 +14561,17 @@
     </row>
     <row r="100" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="6"/>
         <v>Bernstadt</v>
       </c>
       <c r="D100" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="E100" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F100">
         <v>85</v>
@@ -14689,17 +14698,17 @@
     </row>
     <row r="101" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="6"/>
         <v>Loebau</v>
       </c>
       <c r="D101" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="E101" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F101">
         <v>81</v>
@@ -14826,17 +14835,17 @@
     </row>
     <row r="102" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="6"/>
         <v>Dueritz</v>
       </c>
       <c r="D102" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="E102" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F102">
         <v>73</v>
@@ -14963,17 +14972,17 @@
     </row>
     <row r="103" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B103" s="1" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="6"/>
         <v>Weissenberg</v>
       </c>
       <c r="D103" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="E103" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F103">
         <v>154</v>
@@ -15100,17 +15109,17 @@
     </row>
     <row r="104" spans="2:45" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="6"/>
         <v>Zittau</v>
       </c>
       <c r="D104" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="E104" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F104">
         <v>558</v>
@@ -15236,25 +15245,30 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AS1" xr:uid="{F24E769F-0516-B44F-8ED4-BB10FA44B879}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E88AB5-C410-8748-B1FD-5013D32D04ED}">
-  <dimension ref="A1:AM4"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
@@ -15277,10 +15291,10 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="2"/>
+      <c r="V1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
@@ -15294,16 +15308,18 @@
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
-      <c r="AJ1" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AM1" s="2"/>
+      <c r="AO1" s="2"/>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -15320,37 +15336,39 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="2"/>
+      <c r="V2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="2"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2" t="s">
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2" t="s">
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AH2" s="2"/>
-      <c r="AI2" t="s">
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AJ2" s="2"/>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -15408,68 +15426,70 @@
       <c r="S3" t="s">
         <v>23</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="2"/>
+      <c r="V3" t="s">
         <v>25</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>26</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>27</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>28</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>29</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>30</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>32</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>33</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>35</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>34</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>37</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>38</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>40</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>41</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>46</v>
-      </c>
+      <c r="AK3" s="2"/>
       <c r="AL3" t="s">
         <v>45</v>
       </c>
       <c r="AM3" t="s">
         <v>46</v>
       </c>
+      <c r="AN3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -15486,121 +15506,145 @@
         <v>48</v>
       </c>
       <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>176</v>
+      </c>
+      <c r="I4" t="s">
         <v>50</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" t="s">
         <v>51</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
+        <v>178</v>
+      </c>
+      <c r="M4" t="s">
         <v>52</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>53</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
+        <v>180</v>
+      </c>
+      <c r="P4" t="s">
         <v>54</v>
       </c>
-      <c r="L4" t="s">
+      <c r="Q4" t="s">
+        <v>181</v>
+      </c>
+      <c r="R4" t="s">
         <v>55</v>
       </c>
-      <c r="M4" t="s">
+      <c r="S4" t="s">
+        <v>194</v>
+      </c>
+      <c r="T4" t="s">
+        <v>68</v>
+      </c>
+      <c r="U4" t="s">
+        <v>183</v>
+      </c>
+      <c r="V4" t="s">
         <v>56</v>
       </c>
-      <c r="N4" t="s">
+      <c r="W4" t="s">
+        <v>184</v>
+      </c>
+      <c r="X4" t="s">
         <v>57</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Y4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z4" t="s">
         <v>58</v>
       </c>
-      <c r="P4" t="s">
+      <c r="AA4" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB4" t="s">
         <v>59</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="AC4" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD4" t="s">
         <v>60</v>
       </c>
-      <c r="R4" t="s">
+      <c r="AE4" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF4" t="s">
         <v>61</v>
       </c>
-      <c r="S4" t="s">
+      <c r="AG4" t="s">
+        <v>189</v>
+      </c>
+      <c r="AH4" t="s">
         <v>62</v>
       </c>
-      <c r="T4" t="s">
+      <c r="AI4" t="s">
+        <v>190</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>191</v>
+      </c>
+      <c r="AL4" t="s">
         <v>63</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AM4" t="s">
+        <v>192</v>
+      </c>
+      <c r="AN4" t="s">
         <v>64</v>
       </c>
-      <c r="V4" t="s">
-        <v>65</v>
-      </c>
-      <c r="W4" t="s">
-        <v>66</v>
-      </c>
-      <c r="X4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>82</v>
-      </c>
+      <c r="AO4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="E1:F2"/>
     <mergeCell ref="G1:M2"/>
-    <mergeCell ref="N1:T2"/>
+    <mergeCell ref="N1:U2"/>
+    <mergeCell ref="AN1:AO2"/>
+    <mergeCell ref="V2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="V1:AK1"/>
     <mergeCell ref="AL1:AM2"/>
-    <mergeCell ref="U2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="U1:AI1"/>
-    <mergeCell ref="AJ1:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>